<commit_message>
Added CSV test data feature, test data selection yes/no feature
</commit_message>
<xml_diff>
--- a/MevenDemoTest/src/CleartripTestData.xlsx
+++ b/MevenDemoTest/src/CleartripTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13140" windowHeight="3450" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13275" windowHeight="4020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RoundTrip" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="B1:G12"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
   <si>
     <t>Onward Journey date in DD/MM/YYYY</t>
   </si>
@@ -43,9 +42,6 @@
     <t>Kolkata</t>
   </si>
   <si>
-    <t>Bhubaneswar</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -82,15 +78,6 @@
     <t>4</t>
   </si>
   <si>
-    <t>25/12/2019</t>
-  </si>
-  <si>
-    <t>10/09/2020</t>
-  </si>
-  <si>
-    <t>Chennai</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
@@ -121,34 +108,55 @@
     <t>Mandarmoni</t>
   </si>
   <si>
-    <t>01/02/2020</t>
-  </si>
-  <si>
-    <t>05/02/2020</t>
-  </si>
-  <si>
-    <t>08/08/2020</t>
-  </si>
-  <si>
-    <t>Patna</t>
-  </si>
-  <si>
     <t>12/02/2020</t>
   </si>
   <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>Visakhapatnam</t>
+  </si>
+  <si>
     <t>Bhopal</t>
   </si>
   <si>
-    <t>12/03/2020</t>
-  </si>
-  <si>
-    <t>01/04/2020</t>
-  </si>
-  <si>
-    <t>29/04/2020</t>
-  </si>
-  <si>
-    <t>03/05/2020</t>
+    <t>04/04/2020</t>
+  </si>
+  <si>
+    <t>01/05/2020</t>
+  </si>
+  <si>
+    <t>15/02/2020</t>
+  </si>
+  <si>
+    <t>02/03/2020</t>
+  </si>
+  <si>
+    <t>25/03/2020</t>
+  </si>
+  <si>
+    <t>05/04/2020</t>
+  </si>
+  <si>
+    <t>05/12/2020</t>
+  </si>
+  <si>
+    <t>01/01/2021</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Bagdogra</t>
+  </si>
+  <si>
+    <t>01/06/2020</t>
+  </si>
+  <si>
+    <t>To be executed</t>
   </si>
 </sst>
 </file>
@@ -492,25 +500,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="38.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="35.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="18.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8">
+    <row r="1" spans="1:9">
       <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
@@ -532,188 +541,243 @@
       <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="2:8">
+      <c r="I1" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="B4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="B5" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8">
-      <c r="B3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8">
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8">
-      <c r="B5" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576">
+      <formula1>$A$8:$A$9</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" hidden="1" customWidth="1"/>
     <col min="2" max="5" width="20.28515625" style="3"/>
     <col min="6" max="6" width="20.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="B2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="3" t="s">
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>28</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
-      <formula1>$A$2:$A$3</formula1>
+      <formula1>$A$3:$A$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
+      <formula1>$A$6:$A$7</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -725,7 +789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
bug fixes and tuning
</commit_message>
<xml_diff>
--- a/MevenDemoTest/src/CleartripTestData.xlsx
+++ b/MevenDemoTest/src/CleartripTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13275" windowHeight="4020" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13350" windowHeight="5235" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RoundTrip" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="B1:G12"/>
 </workbook>
 </file>
 
@@ -61,103 +60,103 @@
     <t>09/04/2020</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>15/05/2020</t>
+  </si>
+  <si>
+    <t>09/06/2020</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>From date DD/MM/YYYY</t>
+  </si>
+  <si>
+    <t>To date DD/MM/YYYY</t>
+  </si>
+  <si>
+    <t>Travellers</t>
+  </si>
+  <si>
+    <t>2 rooms, 4 adults</t>
+  </si>
+  <si>
+    <t>1 room, 2 adults</t>
+  </si>
+  <si>
+    <t>1 room, 1 adult</t>
+  </si>
+  <si>
+    <t>Digha</t>
+  </si>
+  <si>
+    <t>Puri</t>
+  </si>
+  <si>
+    <t>Mandarmoni</t>
+  </si>
+  <si>
+    <t>12/02/2020</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>Visakhapatnam</t>
+  </si>
+  <si>
+    <t>Bhopal</t>
+  </si>
+  <si>
+    <t>04/04/2020</t>
+  </si>
+  <si>
+    <t>01/05/2020</t>
+  </si>
+  <si>
+    <t>15/02/2020</t>
+  </si>
+  <si>
+    <t>25/03/2020</t>
+  </si>
+  <si>
+    <t>05/12/2020</t>
+  </si>
+  <si>
+    <t>01/01/2021</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Bagdogra</t>
+  </si>
+  <si>
+    <t>01/06/2020</t>
+  </si>
+  <si>
+    <t>To be executed</t>
+  </si>
+  <si>
+    <t>05/04/2021</t>
+  </si>
+  <si>
     <t>04/05/2020</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Bangalore</t>
-  </si>
-  <si>
-    <t>15/05/2020</t>
-  </si>
-  <si>
-    <t>09/06/2020</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>From date DD/MM/YYYY</t>
-  </si>
-  <si>
-    <t>To date DD/MM/YYYY</t>
-  </si>
-  <si>
-    <t>Travellers</t>
-  </si>
-  <si>
-    <t>2 rooms, 4 adults</t>
-  </si>
-  <si>
-    <t>1 room, 2 adults</t>
-  </si>
-  <si>
-    <t>1 room, 1 adult</t>
-  </si>
-  <si>
-    <t>Digha</t>
-  </si>
-  <si>
-    <t>Puri</t>
-  </si>
-  <si>
-    <t>Mandarmoni</t>
-  </si>
-  <si>
-    <t>12/02/2020</t>
-  </si>
-  <si>
-    <t>Hyderabad</t>
-  </si>
-  <si>
-    <t>Visakhapatnam</t>
-  </si>
-  <si>
-    <t>Bhopal</t>
-  </si>
-  <si>
-    <t>04/04/2020</t>
-  </si>
-  <si>
-    <t>01/05/2020</t>
-  </si>
-  <si>
-    <t>15/02/2020</t>
-  </si>
-  <si>
     <t>02/03/2020</t>
-  </si>
-  <si>
-    <t>25/03/2020</t>
-  </si>
-  <si>
-    <t>05/04/2020</t>
-  </si>
-  <si>
-    <t>05/12/2020</t>
-  </si>
-  <si>
-    <t>01/01/2021</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Bagdogra</t>
-  </si>
-  <si>
-    <t>01/06/2020</t>
-  </si>
-  <si>
-    <t>To be executed</t>
   </si>
 </sst>
 </file>
@@ -501,23 +500,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="8" width="14.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -543,47 +535,53 @@
         <v>4</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>43</v>
+      <c r="I2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>8</v>
@@ -595,21 +593,21 @@
         <v>9</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>9</v>
@@ -618,52 +616,42 @@
         <v>8</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>43</v>
+      <c r="I5" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576">
-      <formula1>$A$8:$A$9</formula1>
+      <formula1>$A$2:$A$3</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -674,102 +662,102 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="5" width="20.28515625" style="3"/>
     <col min="6" max="6" width="20.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes for moving excel dropdown to different sheet
</commit_message>
<xml_diff>
--- a/MevenDemoTest/src/CleartripTestData.xlsx
+++ b/MevenDemoTest/src/CleartripTestData.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13350" windowHeight="5235" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18930" windowHeight="6330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RoundTrip" sheetId="1" r:id="rId1"/>
     <sheet name="HotelSearch" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -162,8 +162,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,6 +212,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -258,7 +266,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -290,9 +298,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -324,6 +333,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -499,294 +509,322 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="8" width="14.28515625" style="1"/>
+    <col min="1" max="7" width="14.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="B4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="1" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I5" t="s">
+      <c r="H5" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576">
-      <formula1>$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Sheet3!$A$17:$A$18</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="5" width="20.28515625" style="3"/>
-    <col min="6" max="6" width="20.28515625" style="1"/>
+    <col min="1" max="4" width="20.28515625" style="3"/>
+    <col min="5" max="5" width="20.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="B1" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
-      <formula1>$A$3:$A$4</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
-      <formula1>$A$6:$A$7</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Sheet3!$B$17:$B$19</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Sheet3!$A$17:$A$18</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A16:B19"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17:B19">
+      <formula1>$A$3:$A$4</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
after changes in new flightsearch and logout
</commit_message>
<xml_diff>
--- a/MevenDemoTest/src/CleartripTestData.xlsx
+++ b/MevenDemoTest/src/CleartripTestData.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18930" windowHeight="6330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="12975" windowHeight="4650"/>
   </bookViews>
   <sheets>
     <sheet name="RoundTrip" sheetId="1" r:id="rId1"/>
     <sheet name="HotelSearch" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
+  <oleSize ref="A1:I15"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
   <si>
     <t>Onward Journey date in DD/MM/YYYY</t>
   </si>
@@ -57,21 +58,12 @@
     <t>New Delhi</t>
   </si>
   <si>
-    <t>09/04/2020</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
     <t>Bangalore</t>
   </si>
   <si>
-    <t>15/05/2020</t>
-  </si>
-  <si>
-    <t>09/06/2020</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
@@ -105,9 +97,6 @@
     <t>Mandarmoni</t>
   </si>
   <si>
-    <t>12/02/2020</t>
-  </si>
-  <si>
     <t>Hyderabad</t>
   </si>
   <si>
@@ -117,18 +106,6 @@
     <t>Bhopal</t>
   </si>
   <si>
-    <t>04/04/2020</t>
-  </si>
-  <si>
-    <t>01/05/2020</t>
-  </si>
-  <si>
-    <t>15/02/2020</t>
-  </si>
-  <si>
-    <t>25/03/2020</t>
-  </si>
-  <si>
     <t>05/12/2020</t>
   </si>
   <si>
@@ -141,29 +118,50 @@
     <t>No</t>
   </si>
   <si>
-    <t>Bagdogra</t>
-  </si>
-  <si>
-    <t>01/06/2020</t>
-  </si>
-  <si>
     <t>To be executed</t>
   </si>
   <si>
-    <t>05/04/2021</t>
-  </si>
-  <si>
-    <t>04/05/2020</t>
-  </si>
-  <si>
-    <t>02/03/2020</t>
+    <t>15/08/2020</t>
+  </si>
+  <si>
+    <t>02/09/2020</t>
+  </si>
+  <si>
+    <t>25/10/2020</t>
+  </si>
+  <si>
+    <t>05/11/2020</t>
+  </si>
+  <si>
+    <t>Patna</t>
+  </si>
+  <si>
+    <t>01/09/2020</t>
+  </si>
+  <si>
+    <t>01/10/2020</t>
+  </si>
+  <si>
+    <t>18/09/2020</t>
+  </si>
+  <si>
+    <t>17/11/2020</t>
+  </si>
+  <si>
+    <t>09/11/2020</t>
+  </si>
+  <si>
+    <t>04/12/2020</t>
+  </si>
+  <si>
+    <t>04/10/2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,7 +264,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -298,10 +296,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -333,7 +330,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -509,19 +505,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="7" width="14.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -544,47 +540,47 @@
         <v>4</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>8</v>
@@ -596,21 +592,21 @@
         <v>9</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>9</v>
@@ -619,36 +615,36 @@
         <v>8</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H5" t="s">
-        <v>40</v>
+      <c r="H5" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -670,85 +666,85 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="4" width="20.28515625" style="3"/>
     <col min="5" max="5" width="20.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="E1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -776,46 +772,46 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A16:B19"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.5703125" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="B19" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit test data changes
</commit_message>
<xml_diff>
--- a/MevenDemoTest/src/CleartripTestData.xlsx
+++ b/MevenDemoTest/src/CleartripTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13785" windowHeight="3885" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13785" windowHeight="4785" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RoundTrip" sheetId="1" r:id="rId1"/>
@@ -151,10 +151,10 @@
     <t>04/10/2020</t>
   </si>
   <si>
-    <t>15/0/2020</t>
-  </si>
-  <si>
     <t>02/10/2020</t>
+  </si>
+  <si>
+    <t>15/09/2020</t>
   </si>
 </sst>
 </file>
@@ -670,7 +670,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="15"/>
@@ -701,10 +701,10 @@
         <v>25</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>20</v>

</xml_diff>